<commit_message>
Added MDI fonts and Q2 2022
</commit_message>
<xml_diff>
--- a/data/categories.xlsx
+++ b/data/categories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B662FEFD-AD26-4E84-ACE5-A634CF426DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9AC84D4-749B-447E-8AAC-A6F09AF0A495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Source" sheetId="5" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="Q3 2020-2021" sheetId="14" r:id="rId10"/>
     <sheet name="Q4 2020-2021" sheetId="15" r:id="rId11"/>
     <sheet name="Q1 2021-2022" sheetId="16" r:id="rId12"/>
+    <sheet name="Q2 2021-2022" sheetId="18" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="83">
   <si>
     <t>Alteration of personal data</t>
   </si>
@@ -722,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4757,6 +4758,1205 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5C6BB7-46B3-40E9-86C7-496802ACEB89}">
+  <dimension ref="A1:X25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9" style="26" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9" style="26" customWidth="1"/>
+    <col min="24" max="24" width="6.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="9.140625" style="26"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B1" s="26" t="str">
+        <f>'ICO Bodies'!B2</f>
+        <v>Central Government</v>
+      </c>
+      <c r="C1" s="26" t="str">
+        <f>'ICO Bodies'!B3</f>
+        <v>Charitable and voluntary</v>
+      </c>
+      <c r="D1" s="26" t="str">
+        <f>'ICO Bodies'!B4</f>
+        <v>Education and childcare</v>
+      </c>
+      <c r="E1" s="26" t="str">
+        <f>'ICO Bodies'!B5</f>
+        <v>Finance, insurance and credit</v>
+      </c>
+      <c r="F1" s="26" t="str">
+        <f>'ICO Bodies'!B6</f>
+        <v>General business</v>
+      </c>
+      <c r="G1" s="26" t="str">
+        <f>'ICO Bodies'!B7</f>
+        <v>Health</v>
+      </c>
+      <c r="H1" s="26" t="str">
+        <f>'ICO Bodies'!B8</f>
+        <v>Justice</v>
+      </c>
+      <c r="I1" s="26" t="str">
+        <f>'ICO Bodies'!B9</f>
+        <v>Land or property services</v>
+      </c>
+      <c r="J1" s="26" t="str">
+        <f>'ICO Bodies'!B10</f>
+        <v>Legal</v>
+      </c>
+      <c r="K1" s="26" t="str">
+        <f>'ICO Bodies'!B11</f>
+        <v>Local government</v>
+      </c>
+      <c r="L1" s="26" t="str">
+        <f>'ICO Bodies'!B12</f>
+        <v>Marketing</v>
+      </c>
+      <c r="M1" s="26" t="str">
+        <f>'ICO Bodies'!B13</f>
+        <v>Media</v>
+      </c>
+      <c r="N1" s="26" t="str">
+        <f>'ICO Bodies'!B14</f>
+        <v>Membership association</v>
+      </c>
+      <c r="O1" s="26" t="str">
+        <f>'ICO Bodies'!B15</f>
+        <v>Online Technology and Telecoms</v>
+      </c>
+      <c r="P1" s="26" t="str">
+        <f>'ICO Bodies'!B16</f>
+        <v>Political</v>
+      </c>
+      <c r="Q1" s="26" t="str">
+        <f>'ICO Bodies'!B17</f>
+        <v>Regulators</v>
+      </c>
+      <c r="R1" s="26" t="str">
+        <f>'ICO Bodies'!B18</f>
+        <v>Religious</v>
+      </c>
+      <c r="S1" s="26" t="str">
+        <f>'ICO Bodies'!B19</f>
+        <v>Retail and manufacture</v>
+      </c>
+      <c r="T1" s="26" t="str">
+        <f>'ICO Bodies'!B20</f>
+        <v>Social care</v>
+      </c>
+      <c r="U1" s="26" t="str">
+        <f>'ICO Bodies'!B21</f>
+        <v>Transport and leisure</v>
+      </c>
+      <c r="V1" s="26" t="str">
+        <f>'ICO Bodies'!B22</f>
+        <v>Utilities</v>
+      </c>
+      <c r="W1" s="26" t="str">
+        <f>'ICO Bodies'!B23</f>
+        <v>Unassigned</v>
+      </c>
+      <c r="X1" s="26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="str">
+        <f>'ICO Categories'!B2</f>
+        <v>Alteration of personal data</v>
+      </c>
+      <c r="D2" s="26">
+        <v>1</v>
+      </c>
+      <c r="E2" s="26">
+        <v>2</v>
+      </c>
+      <c r="G2" s="26">
+        <v>4</v>
+      </c>
+      <c r="K2" s="26">
+        <v>1</v>
+      </c>
+      <c r="O2" s="26">
+        <v>1</v>
+      </c>
+      <c r="V2" s="26">
+        <v>1</v>
+      </c>
+      <c r="X2" s="26">
+        <f>SUM(B2:W2)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="str">
+        <f>'ICO Categories'!B3</f>
+        <v>Data emailed to incorrect recipient</v>
+      </c>
+      <c r="B3" s="26">
+        <v>9</v>
+      </c>
+      <c r="C3" s="26">
+        <v>19</v>
+      </c>
+      <c r="D3" s="26">
+        <v>78</v>
+      </c>
+      <c r="E3" s="26">
+        <v>33</v>
+      </c>
+      <c r="F3" s="26">
+        <v>12</v>
+      </c>
+      <c r="G3" s="26">
+        <v>63</v>
+      </c>
+      <c r="H3" s="26">
+        <v>2</v>
+      </c>
+      <c r="I3" s="26">
+        <v>30</v>
+      </c>
+      <c r="J3" s="26">
+        <v>72</v>
+      </c>
+      <c r="K3" s="26">
+        <v>32</v>
+      </c>
+      <c r="N3" s="26">
+        <v>3</v>
+      </c>
+      <c r="O3" s="26">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="26">
+        <v>6</v>
+      </c>
+      <c r="S3" s="26">
+        <v>16</v>
+      </c>
+      <c r="T3" s="26">
+        <v>12</v>
+      </c>
+      <c r="U3" s="26">
+        <v>2</v>
+      </c>
+      <c r="V3" s="26">
+        <v>3</v>
+      </c>
+      <c r="X3" s="26">
+        <f t="shared" ref="X3:X24" si="0">SUM(B3:W3)</f>
+        <v>397</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="str">
+        <f>'ICO Categories'!B4</f>
+        <v>Data of wrong data subject shown in client portal</v>
+      </c>
+      <c r="B4" s="26">
+        <v>3</v>
+      </c>
+      <c r="C4" s="26">
+        <v>1</v>
+      </c>
+      <c r="D4" s="26">
+        <v>5</v>
+      </c>
+      <c r="E4" s="26">
+        <v>2</v>
+      </c>
+      <c r="F4" s="26">
+        <v>1</v>
+      </c>
+      <c r="G4" s="26">
+        <v>5</v>
+      </c>
+      <c r="I4" s="26">
+        <v>2</v>
+      </c>
+      <c r="K4" s="26">
+        <v>3</v>
+      </c>
+      <c r="N4" s="26">
+        <v>1</v>
+      </c>
+      <c r="S4" s="26">
+        <v>3</v>
+      </c>
+      <c r="X4" s="26">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="str">
+        <f>'ICO Categories'!B5</f>
+        <v>Data posted or faxed to incorrect recipient</v>
+      </c>
+      <c r="B5" s="26">
+        <v>11</v>
+      </c>
+      <c r="C5" s="26">
+        <v>6</v>
+      </c>
+      <c r="D5" s="26">
+        <v>14</v>
+      </c>
+      <c r="E5" s="26">
+        <v>23</v>
+      </c>
+      <c r="F5" s="26">
+        <v>2</v>
+      </c>
+      <c r="G5" s="26">
+        <v>56</v>
+      </c>
+      <c r="H5" s="26">
+        <v>3</v>
+      </c>
+      <c r="I5" s="26">
+        <v>9</v>
+      </c>
+      <c r="J5" s="26">
+        <v>24</v>
+      </c>
+      <c r="K5" s="26">
+        <v>28</v>
+      </c>
+      <c r="N5" s="26">
+        <v>1</v>
+      </c>
+      <c r="S5" s="26">
+        <v>11</v>
+      </c>
+      <c r="T5" s="26">
+        <v>1</v>
+      </c>
+      <c r="U5" s="26">
+        <v>1</v>
+      </c>
+      <c r="V5" s="26">
+        <v>2</v>
+      </c>
+      <c r="X5" s="26">
+        <f t="shared" si="0"/>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="str">
+        <f>'ICO Categories'!B6</f>
+        <v>Failure to redact</v>
+      </c>
+      <c r="B6" s="26">
+        <v>5</v>
+      </c>
+      <c r="C6" s="26">
+        <v>5</v>
+      </c>
+      <c r="D6" s="26">
+        <v>16</v>
+      </c>
+      <c r="E6" s="26">
+        <v>1</v>
+      </c>
+      <c r="F6" s="26">
+        <v>1</v>
+      </c>
+      <c r="G6" s="26">
+        <v>8</v>
+      </c>
+      <c r="H6" s="26">
+        <v>4</v>
+      </c>
+      <c r="I6" s="26">
+        <v>2</v>
+      </c>
+      <c r="J6" s="26">
+        <v>13</v>
+      </c>
+      <c r="K6" s="26">
+        <v>42</v>
+      </c>
+      <c r="O6" s="26">
+        <v>1</v>
+      </c>
+      <c r="R6" s="26">
+        <v>1</v>
+      </c>
+      <c r="S6" s="26">
+        <v>1</v>
+      </c>
+      <c r="T6" s="26">
+        <v>2</v>
+      </c>
+      <c r="X6" s="26">
+        <f t="shared" si="0"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="str">
+        <f>'ICO Categories'!B7</f>
+        <v>Failure to use bcc</v>
+      </c>
+      <c r="B7" s="26">
+        <v>2</v>
+      </c>
+      <c r="C7" s="26">
+        <v>7</v>
+      </c>
+      <c r="D7" s="26">
+        <v>11</v>
+      </c>
+      <c r="E7" s="26">
+        <v>4</v>
+      </c>
+      <c r="F7" s="26">
+        <v>6</v>
+      </c>
+      <c r="G7" s="26">
+        <v>10</v>
+      </c>
+      <c r="I7" s="26">
+        <v>7</v>
+      </c>
+      <c r="J7" s="26">
+        <v>1</v>
+      </c>
+      <c r="K7" s="26">
+        <v>4</v>
+      </c>
+      <c r="M7" s="26">
+        <v>1</v>
+      </c>
+      <c r="N7" s="26">
+        <v>4</v>
+      </c>
+      <c r="O7" s="26">
+        <v>2</v>
+      </c>
+      <c r="S7" s="26">
+        <v>7</v>
+      </c>
+      <c r="T7" s="26">
+        <v>1</v>
+      </c>
+      <c r="U7" s="26">
+        <v>4</v>
+      </c>
+      <c r="V7" s="26">
+        <v>1</v>
+      </c>
+      <c r="X7" s="26">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="str">
+        <f>'ICO Categories'!B8</f>
+        <v>Incorrect disposal of hardware</v>
+      </c>
+      <c r="C8" s="26">
+        <v>1</v>
+      </c>
+      <c r="G8" s="26">
+        <v>1</v>
+      </c>
+      <c r="N8" s="26">
+        <v>2</v>
+      </c>
+      <c r="X8" s="26">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="str">
+        <f>'ICO Categories'!B9</f>
+        <v>Incorrect disposal of paperwork</v>
+      </c>
+      <c r="B9" s="26">
+        <v>1</v>
+      </c>
+      <c r="C9" s="26">
+        <v>1</v>
+      </c>
+      <c r="D9" s="26">
+        <v>2</v>
+      </c>
+      <c r="G9" s="26">
+        <v>3</v>
+      </c>
+      <c r="J9" s="26">
+        <v>1</v>
+      </c>
+      <c r="K9" s="26">
+        <v>1</v>
+      </c>
+      <c r="T9" s="26">
+        <v>2</v>
+      </c>
+      <c r="X9" s="26">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="str">
+        <f>'ICO Categories'!B10</f>
+        <v>Loss/theft of device containing personal data</v>
+      </c>
+      <c r="C10" s="26">
+        <v>4</v>
+      </c>
+      <c r="D10" s="26">
+        <v>8</v>
+      </c>
+      <c r="E10" s="26">
+        <v>3</v>
+      </c>
+      <c r="F10" s="26">
+        <v>1</v>
+      </c>
+      <c r="G10" s="26">
+        <v>8</v>
+      </c>
+      <c r="H10" s="26">
+        <v>2</v>
+      </c>
+      <c r="I10" s="26">
+        <v>1</v>
+      </c>
+      <c r="J10" s="26">
+        <v>6</v>
+      </c>
+      <c r="K10" s="26">
+        <v>6</v>
+      </c>
+      <c r="O10" s="26">
+        <v>1</v>
+      </c>
+      <c r="S10" s="26">
+        <v>2</v>
+      </c>
+      <c r="T10" s="26">
+        <v>1</v>
+      </c>
+      <c r="U10" s="26">
+        <v>2</v>
+      </c>
+      <c r="X10" s="26">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="str">
+        <f>'ICO Categories'!B11</f>
+        <v>Loss/theft of paperwork or data left in insecure location</v>
+      </c>
+      <c r="B11" s="26">
+        <v>6</v>
+      </c>
+      <c r="C11" s="26">
+        <v>20</v>
+      </c>
+      <c r="D11" s="26">
+        <v>10</v>
+      </c>
+      <c r="E11" s="26">
+        <v>5</v>
+      </c>
+      <c r="F11" s="26">
+        <v>4</v>
+      </c>
+      <c r="G11" s="26">
+        <v>52</v>
+      </c>
+      <c r="H11" s="26">
+        <v>10</v>
+      </c>
+      <c r="I11" s="26">
+        <v>6</v>
+      </c>
+      <c r="J11" s="26">
+        <v>11</v>
+      </c>
+      <c r="K11" s="26">
+        <v>11</v>
+      </c>
+      <c r="M11" s="26">
+        <v>2</v>
+      </c>
+      <c r="N11" s="26">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="26">
+        <v>1</v>
+      </c>
+      <c r="S11" s="26">
+        <v>5</v>
+      </c>
+      <c r="T11" s="26">
+        <v>16</v>
+      </c>
+      <c r="U11" s="26">
+        <v>3</v>
+      </c>
+      <c r="X11" s="26">
+        <f t="shared" si="0"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="str">
+        <f>'ICO Categories'!B12</f>
+        <v>Not Provided</v>
+      </c>
+      <c r="C12" s="26">
+        <v>2</v>
+      </c>
+      <c r="D12" s="26">
+        <v>12</v>
+      </c>
+      <c r="E12" s="26">
+        <v>8</v>
+      </c>
+      <c r="F12" s="26">
+        <v>3</v>
+      </c>
+      <c r="G12" s="26">
+        <v>14</v>
+      </c>
+      <c r="J12" s="26">
+        <v>9</v>
+      </c>
+      <c r="K12" s="26">
+        <v>6</v>
+      </c>
+      <c r="N12" s="26">
+        <v>1</v>
+      </c>
+      <c r="S12" s="26">
+        <v>6</v>
+      </c>
+      <c r="T12" s="26">
+        <v>1</v>
+      </c>
+      <c r="U12" s="26">
+        <v>2</v>
+      </c>
+      <c r="X12" s="26">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="str">
+        <f>'ICO Categories'!B13</f>
+        <v>Other non-cyber incident</v>
+      </c>
+      <c r="B13" s="26">
+        <v>14</v>
+      </c>
+      <c r="C13" s="26">
+        <v>19</v>
+      </c>
+      <c r="D13" s="26">
+        <v>59</v>
+      </c>
+      <c r="E13" s="26">
+        <v>23</v>
+      </c>
+      <c r="F13" s="26">
+        <v>9</v>
+      </c>
+      <c r="G13" s="26">
+        <v>99</v>
+      </c>
+      <c r="H13" s="26">
+        <v>13</v>
+      </c>
+      <c r="I13" s="26">
+        <v>18</v>
+      </c>
+      <c r="J13" s="26">
+        <v>9</v>
+      </c>
+      <c r="K13" s="26">
+        <v>40</v>
+      </c>
+      <c r="M13" s="26">
+        <v>1</v>
+      </c>
+      <c r="N13" s="26">
+        <v>1</v>
+      </c>
+      <c r="O13" s="26">
+        <v>10</v>
+      </c>
+      <c r="Q13" s="26">
+        <v>4</v>
+      </c>
+      <c r="R13" s="26">
+        <v>2</v>
+      </c>
+      <c r="S13" s="26">
+        <v>15</v>
+      </c>
+      <c r="T13" s="26">
+        <v>6</v>
+      </c>
+      <c r="U13" s="26">
+        <v>10</v>
+      </c>
+      <c r="V13" s="26">
+        <v>1</v>
+      </c>
+      <c r="X13" s="26">
+        <f t="shared" si="0"/>
+        <v>353</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="str">
+        <f>'ICO Categories'!B14</f>
+        <v>Unauthorised access (non-cyber)</v>
+      </c>
+      <c r="B14" s="26">
+        <v>2</v>
+      </c>
+      <c r="C14" s="26">
+        <v>5</v>
+      </c>
+      <c r="D14" s="26">
+        <v>24</v>
+      </c>
+      <c r="E14" s="26">
+        <v>13</v>
+      </c>
+      <c r="F14" s="26">
+        <v>11</v>
+      </c>
+      <c r="G14" s="26">
+        <v>67</v>
+      </c>
+      <c r="H14" s="26">
+        <v>3</v>
+      </c>
+      <c r="I14" s="26">
+        <v>10</v>
+      </c>
+      <c r="J14" s="26">
+        <v>6</v>
+      </c>
+      <c r="K14" s="26">
+        <v>23</v>
+      </c>
+      <c r="M14" s="26">
+        <v>2</v>
+      </c>
+      <c r="N14" s="26">
+        <v>2</v>
+      </c>
+      <c r="O14" s="26">
+        <v>2</v>
+      </c>
+      <c r="P14" s="26">
+        <v>1</v>
+      </c>
+      <c r="R14" s="26">
+        <v>1</v>
+      </c>
+      <c r="S14" s="26">
+        <v>13</v>
+      </c>
+      <c r="T14" s="26">
+        <v>11</v>
+      </c>
+      <c r="U14" s="26">
+        <v>10</v>
+      </c>
+      <c r="V14" s="26">
+        <v>3</v>
+      </c>
+      <c r="X14" s="26">
+        <f t="shared" si="0"/>
+        <v>209</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="str">
+        <f>'ICO Categories'!B15</f>
+        <v>Verbal disclosure of personal data</v>
+      </c>
+      <c r="B15" s="26">
+        <v>1</v>
+      </c>
+      <c r="C15" s="26">
+        <v>5</v>
+      </c>
+      <c r="D15" s="26">
+        <v>9</v>
+      </c>
+      <c r="E15" s="26">
+        <v>6</v>
+      </c>
+      <c r="F15" s="26">
+        <v>1</v>
+      </c>
+      <c r="G15" s="26">
+        <v>12</v>
+      </c>
+      <c r="H15" s="26">
+        <v>1</v>
+      </c>
+      <c r="I15" s="26">
+        <v>13</v>
+      </c>
+      <c r="K15" s="26">
+        <v>9</v>
+      </c>
+      <c r="N15" s="26">
+        <v>1</v>
+      </c>
+      <c r="S15" s="26">
+        <v>2</v>
+      </c>
+      <c r="T15" s="26">
+        <v>3</v>
+      </c>
+      <c r="U15" s="26">
+        <v>1</v>
+      </c>
+      <c r="V15" s="26">
+        <v>4</v>
+      </c>
+      <c r="X15" s="26">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="str">
+        <f>'ICO Categories'!B16</f>
+        <v>Brute Force</v>
+      </c>
+      <c r="C16" s="26">
+        <v>3</v>
+      </c>
+      <c r="D16" s="26">
+        <v>1</v>
+      </c>
+      <c r="E16" s="26">
+        <v>4</v>
+      </c>
+      <c r="F16" s="26">
+        <v>3</v>
+      </c>
+      <c r="G16" s="26">
+        <v>1</v>
+      </c>
+      <c r="I16" s="26">
+        <v>1</v>
+      </c>
+      <c r="J16" s="26">
+        <v>2</v>
+      </c>
+      <c r="K16" s="26">
+        <v>1</v>
+      </c>
+      <c r="N16" s="26">
+        <v>1</v>
+      </c>
+      <c r="O16" s="26">
+        <v>2</v>
+      </c>
+      <c r="S16" s="26">
+        <v>8</v>
+      </c>
+      <c r="U16" s="26">
+        <v>1</v>
+      </c>
+      <c r="X16" s="26">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17" s="26" t="str">
+        <f>'ICO Categories'!B17</f>
+        <v>Denial of service</v>
+      </c>
+      <c r="E17" s="26">
+        <v>3</v>
+      </c>
+      <c r="O17" s="26">
+        <v>1</v>
+      </c>
+      <c r="X17" s="26">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="str">
+        <f>'ICO Categories'!B18</f>
+        <v>Hardware/software misconfiguration</v>
+      </c>
+      <c r="B18" s="26">
+        <v>1</v>
+      </c>
+      <c r="C18" s="26">
+        <v>1</v>
+      </c>
+      <c r="D18" s="26">
+        <v>6</v>
+      </c>
+      <c r="E18" s="26">
+        <v>11</v>
+      </c>
+      <c r="F18" s="26">
+        <v>5</v>
+      </c>
+      <c r="G18" s="26">
+        <v>8</v>
+      </c>
+      <c r="I18" s="26">
+        <v>3</v>
+      </c>
+      <c r="J18" s="26">
+        <v>1</v>
+      </c>
+      <c r="K18" s="26">
+        <v>2</v>
+      </c>
+      <c r="M18" s="26">
+        <v>1</v>
+      </c>
+      <c r="N18" s="26">
+        <v>1</v>
+      </c>
+      <c r="O18" s="26">
+        <v>7</v>
+      </c>
+      <c r="S18" s="26">
+        <v>5</v>
+      </c>
+      <c r="T18" s="26">
+        <v>1</v>
+      </c>
+      <c r="U18" s="26">
+        <v>3</v>
+      </c>
+      <c r="X18" s="26">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="str">
+        <f>'ICO Categories'!B19</f>
+        <v>Malware</v>
+      </c>
+      <c r="E19" s="26">
+        <v>6</v>
+      </c>
+      <c r="I19" s="26">
+        <v>1</v>
+      </c>
+      <c r="J19" s="26">
+        <v>3</v>
+      </c>
+      <c r="K19" s="26">
+        <v>2</v>
+      </c>
+      <c r="N19" s="26">
+        <v>1</v>
+      </c>
+      <c r="S19" s="26">
+        <v>10</v>
+      </c>
+      <c r="X19" s="26">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A20" s="26" t="str">
+        <f>'ICO Categories'!B20</f>
+        <v>Other cyber incident</v>
+      </c>
+      <c r="B20" s="26">
+        <v>1</v>
+      </c>
+      <c r="C20" s="26">
+        <v>4</v>
+      </c>
+      <c r="D20" s="26">
+        <v>4</v>
+      </c>
+      <c r="E20" s="26">
+        <v>9</v>
+      </c>
+      <c r="F20" s="26">
+        <v>6</v>
+      </c>
+      <c r="G20" s="26">
+        <v>4</v>
+      </c>
+      <c r="I20" s="26">
+        <v>2</v>
+      </c>
+      <c r="K20" s="26">
+        <v>1</v>
+      </c>
+      <c r="L20" s="26">
+        <v>1</v>
+      </c>
+      <c r="N20" s="26">
+        <v>2</v>
+      </c>
+      <c r="O20" s="26">
+        <v>4</v>
+      </c>
+      <c r="S20" s="26">
+        <v>9</v>
+      </c>
+      <c r="U20" s="26">
+        <v>4</v>
+      </c>
+      <c r="X20" s="26">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="str">
+        <f>'ICO Categories'!B21</f>
+        <v>Phishing</v>
+      </c>
+      <c r="B21" s="26">
+        <v>1</v>
+      </c>
+      <c r="C21" s="26">
+        <v>27</v>
+      </c>
+      <c r="D21" s="26">
+        <v>27</v>
+      </c>
+      <c r="E21" s="26">
+        <v>41</v>
+      </c>
+      <c r="F21" s="26">
+        <v>33</v>
+      </c>
+      <c r="G21" s="26">
+        <v>9</v>
+      </c>
+      <c r="I21" s="26">
+        <v>22</v>
+      </c>
+      <c r="J21" s="26">
+        <v>31</v>
+      </c>
+      <c r="K21" s="26">
+        <v>7</v>
+      </c>
+      <c r="L21" s="26">
+        <v>2</v>
+      </c>
+      <c r="N21" s="26">
+        <v>6</v>
+      </c>
+      <c r="O21" s="26">
+        <v>6</v>
+      </c>
+      <c r="R21" s="26">
+        <v>1</v>
+      </c>
+      <c r="S21" s="26">
+        <v>43</v>
+      </c>
+      <c r="T21" s="26">
+        <v>5</v>
+      </c>
+      <c r="U21" s="26">
+        <v>7</v>
+      </c>
+      <c r="X21" s="26">
+        <f t="shared" si="0"/>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="str">
+        <f>'ICO Categories'!B22</f>
+        <v>Ransomware</v>
+      </c>
+      <c r="B22" s="26">
+        <v>1</v>
+      </c>
+      <c r="C22" s="26">
+        <v>5</v>
+      </c>
+      <c r="D22" s="26">
+        <v>17</v>
+      </c>
+      <c r="E22" s="26">
+        <v>57</v>
+      </c>
+      <c r="F22" s="26">
+        <v>17</v>
+      </c>
+      <c r="G22" s="26">
+        <v>7</v>
+      </c>
+      <c r="H22" s="26">
+        <v>2</v>
+      </c>
+      <c r="I22" s="26">
+        <v>14</v>
+      </c>
+      <c r="J22" s="26">
+        <v>17</v>
+      </c>
+      <c r="K22" s="26">
+        <v>32</v>
+      </c>
+      <c r="N22" s="26">
+        <v>1</v>
+      </c>
+      <c r="O22" s="26">
+        <v>5</v>
+      </c>
+      <c r="R22" s="26">
+        <v>1</v>
+      </c>
+      <c r="S22" s="26">
+        <v>34</v>
+      </c>
+      <c r="T22" s="26">
+        <v>1</v>
+      </c>
+      <c r="U22" s="26">
+        <v>7</v>
+      </c>
+      <c r="V22" s="26">
+        <v>1</v>
+      </c>
+      <c r="X22" s="26">
+        <f t="shared" si="0"/>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="str">
+        <f>'ICO Categories'!B23</f>
+        <v>Unauthorised access (cyber)</v>
+      </c>
+      <c r="B23" s="26">
+        <v>2</v>
+      </c>
+      <c r="C23" s="26">
+        <v>1</v>
+      </c>
+      <c r="D23" s="26">
+        <v>9</v>
+      </c>
+      <c r="E23" s="26">
+        <v>5</v>
+      </c>
+      <c r="F23" s="26">
+        <v>6</v>
+      </c>
+      <c r="G23" s="26">
+        <v>4</v>
+      </c>
+      <c r="I23" s="26">
+        <v>2</v>
+      </c>
+      <c r="J23" s="26">
+        <v>1</v>
+      </c>
+      <c r="L23" s="26">
+        <v>1</v>
+      </c>
+      <c r="M23" s="26">
+        <v>1</v>
+      </c>
+      <c r="N23" s="26">
+        <v>1</v>
+      </c>
+      <c r="O23" s="26">
+        <v>8</v>
+      </c>
+      <c r="S23" s="26">
+        <v>19</v>
+      </c>
+      <c r="U23" s="26">
+        <v>4</v>
+      </c>
+      <c r="V23" s="26">
+        <v>1</v>
+      </c>
+      <c r="X23" s="26">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="str">
+        <f>'ICO Categories'!B24</f>
+        <v>Cryptographic flaw</v>
+      </c>
+      <c r="X24" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X25" s="26">
+        <f>SUM(X2:X24)</f>
+        <v>2431</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D24"/>

</xml_diff>

<commit_message>
Added categories and body seeds
Now you can add the bodies and categories as a seed.
</commit_message>
<xml_diff>
--- a/data/categories.xlsx
+++ b/data/categories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9AC84D4-749B-447E-8AAC-A6F09AF0A495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4EBEBE-C670-4AA9-B577-56A11BCA4651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Source" sheetId="5" r:id="rId1"/>
@@ -779,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="X27" sqref="X27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4762,7 +4762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5C6BB7-46B3-40E9-86C7-496802ACEB89}">
   <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -5961,8 +5961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6320,7 +6320,7 @@
   <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B23" sqref="B2:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>